<commit_message>
First Simulation Draft Working
</commit_message>
<xml_diff>
--- a/Doc/InstructionSet.xlsx
+++ b/Doc/InstructionSet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pschilk\Google Drive\psMCU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pschilk\home\Repos\psMCU\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75CEBAB-1B02-47D0-8899-FAAF91313324}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C50375-FFC1-4879-8CBB-01ECF1F7CB45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4752" yWindow="3012" windowWidth="8820" windowHeight="5748" xr2:uid="{2EEA8C3F-B9BC-45D7-931E-0DD5ED819EBA}"/>
+    <workbookView xWindow="6144" yWindow="4728" windowWidth="8820" windowHeight="5748" xr2:uid="{2EEA8C3F-B9BC-45D7-931E-0DD5ED819EBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="59">
   <si>
     <t>Instruction</t>
   </si>
@@ -126,9 +126,6 @@
     <t>RTRN</t>
   </si>
   <si>
-    <t>COPY A/B B/A</t>
-  </si>
-  <si>
     <t>WriteRamDyn</t>
   </si>
   <si>
@@ -151,13 +148,73 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Mnm.</t>
+  </si>
+  <si>
+    <t>JMP</t>
+  </si>
+  <si>
+    <t>CALL</t>
+  </si>
+  <si>
+    <t>TB[S/R]R</t>
+  </si>
+  <si>
+    <t>TB[S/R]M</t>
+  </si>
+  <si>
+    <t>[AND/OR/XOR](L)</t>
+  </si>
+  <si>
+    <t>LIT</t>
+  </si>
+  <si>
+    <t>ADD(L)</t>
+  </si>
+  <si>
+    <t>COPY A/B</t>
+  </si>
+  <si>
+    <t>CPY</t>
+  </si>
+  <si>
+    <t>NOTA</t>
+  </si>
+  <si>
+    <t>KOMPB</t>
+  </si>
+  <si>
+    <t>SUB</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>SWP</t>
+  </si>
+  <si>
+    <t>SHFT[R/L](L)</t>
+  </si>
+  <si>
+    <t>RD[A/B]</t>
+  </si>
+  <si>
+    <t>WT[A/B]</t>
+  </si>
+  <si>
+    <t>WTD</t>
+  </si>
+  <si>
+    <t>RDD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,15 +222,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,14 +260,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -415,11 +459,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -438,9 +502,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -469,6 +530,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -494,7 +564,63 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="61">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1176,297 +1302,346 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5890C83-178E-4CA4-8BC2-8D6953071DB1}">
-  <dimension ref="A1:S27"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.77734375" style="7" customWidth="1"/>
-    <col min="3" max="16" width="4.77734375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="4.77734375" style="3" customWidth="1"/>
-    <col min="18" max="18" width="49.44140625" customWidth="1"/>
-    <col min="19" max="19" width="63.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="4.77734375" style="7" customWidth="1"/>
+    <col min="4" max="17" width="4.77734375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="4.77734375" style="3" customWidth="1"/>
+    <col min="19" max="19" width="49.44140625" customWidth="1"/>
+    <col min="20" max="20" width="63.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12">
+    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="11">
         <v>15</v>
       </c>
-      <c r="C1" s="13">
+      <c r="D1" s="12">
         <v>14</v>
       </c>
-      <c r="D1" s="14">
+      <c r="E1" s="13">
         <v>13</v>
       </c>
-      <c r="E1" s="14">
+      <c r="F1" s="13">
         <v>12</v>
       </c>
-      <c r="F1" s="14">
+      <c r="G1" s="13">
         <v>11</v>
       </c>
-      <c r="G1" s="14">
+      <c r="H1" s="13">
         <v>10</v>
       </c>
-      <c r="H1" s="14">
+      <c r="I1" s="13">
         <v>9</v>
       </c>
-      <c r="I1" s="15">
+      <c r="J1" s="14">
         <v>8</v>
       </c>
-      <c r="J1" s="15">
+      <c r="K1" s="14">
         <v>7</v>
       </c>
-      <c r="K1" s="15">
+      <c r="L1" s="14">
         <v>6</v>
       </c>
-      <c r="L1" s="15">
+      <c r="M1" s="14">
         <v>5</v>
       </c>
-      <c r="M1" s="15">
+      <c r="N1" s="14">
         <v>4</v>
       </c>
-      <c r="N1" s="15">
+      <c r="O1" s="14">
         <v>3</v>
       </c>
-      <c r="O1" s="15">
+      <c r="P1" s="14">
         <v>2</v>
       </c>
-      <c r="P1" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q1" s="16">
-        <v>0</v>
-      </c>
-      <c r="R1" s="17" t="s">
+      <c r="Q1" s="14">
+        <v>1</v>
+      </c>
+      <c r="R1" s="15">
+        <v>0</v>
+      </c>
+      <c r="S1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="T1" s="17" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="23" t="s">
+      <c r="B2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" t="s">
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="26"/>
+      <c r="S2" t="s">
         <v>5</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7">
-        <v>1</v>
+      <c r="B3" s="20" t="s">
+        <v>41</v>
       </c>
       <c r="C3" s="7">
-        <v>0</v>
-      </c>
-      <c r="D3" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" t="s">
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="24"/>
+      <c r="S3" t="s">
         <v>6</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="7">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
+      <c r="B4" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="G4" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="21" t="s">
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" t="s">
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="24"/>
+      <c r="S4" t="s">
         <v>11</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="7">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="G5" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="7">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="7">
         <v>0</v>
       </c>
       <c r="D6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="G6" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="25"/>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="27"/>
+      <c r="J6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="K6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="20"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="22"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="7">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="7">
         <v>0</v>
       </c>
       <c r="D7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="2">
-        <v>1</v>
-      </c>
-      <c r="H7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="J7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="22"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="24"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="7">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="7">
         <v>0</v>
       </c>
       <c r="D8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
@@ -1474,36 +1649,39 @@
       <c r="G8" s="2">
         <v>0</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="J8" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="22"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="24"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="7">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="7">
         <v>0</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
@@ -1511,476 +1689,520 @@
       <c r="G9" s="2">
         <v>1</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="20"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="22"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="7">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="7">
         <v>0</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
       </c>
       <c r="E10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
       </c>
       <c r="G10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="2">
-        <v>1</v>
-      </c>
-      <c r="I10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="K10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O10" s="19" t="s">
+      <c r="L10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="20"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="22"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="7">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="7">
         <v>0</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
       </c>
       <c r="E11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
       </c>
       <c r="G11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="2">
         <v>0</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="K11" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="20"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="22"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="7">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1</v>
-      </c>
-      <c r="H12" s="2">
-        <v>1</v>
-      </c>
-      <c r="I12" s="6" t="s">
+      <c r="B13" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q12" s="3" t="s">
-        <v>39</v>
+      <c r="B17" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="7">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2">
-        <v>1</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q13" s="3" t="s">
-        <v>39</v>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="7">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2">
-        <v>1</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q14" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="7">
-        <v>0</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="7">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2">
-        <v>1</v>
-      </c>
-      <c r="H16" s="2">
-        <v>1</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="7">
-        <v>0</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2">
-        <v>1</v>
-      </c>
-      <c r="G17" s="2">
-        <v>1</v>
-      </c>
-      <c r="H17" s="2">
-        <v>0</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q17" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="7">
-        <v>0</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2">
-        <v>1</v>
-      </c>
-      <c r="G18" s="2">
-        <v>0</v>
-      </c>
-      <c r="H18" s="2">
-        <v>1</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q18" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="7">
-        <v>0</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="B19" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="7">
         <v>0</v>
       </c>
       <c r="D19" s="2">
@@ -1990,50 +2212,53 @@
         <v>0</v>
       </c>
       <c r="F19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="2">
         <v>0</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>39</v>
+      <c r="I19" s="2">
+        <v>0</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q19" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="7">
-        <v>0</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="B20" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="7">
         <v>0</v>
       </c>
       <c r="D20" s="2">
@@ -2046,47 +2271,50 @@
         <v>0</v>
       </c>
       <c r="G20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="2">
         <v>1</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>39</v>
+      <c r="I20" s="2">
+        <v>1</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q20" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="7">
-        <v>0</v>
-      </c>
-      <c r="C21" s="2">
+      <c r="B21" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="7">
         <v>0</v>
       </c>
       <c r="D21" s="2">
@@ -2099,47 +2327,50 @@
         <v>0</v>
       </c>
       <c r="G21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="2">
-        <v>0</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>39</v>
+        <v>1</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q21" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="7">
-        <v>0</v>
-      </c>
-      <c r="C22" s="2">
+      <c r="B22" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="7">
         <v>0</v>
       </c>
       <c r="D22" s="2">
@@ -2155,44 +2386,47 @@
         <v>0</v>
       </c>
       <c r="H22" s="2">
-        <v>1</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>39</v>
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <v>1</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q22" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="7">
-        <v>0</v>
-      </c>
-      <c r="C23" s="2">
+      <c r="B23" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="7">
         <v>0</v>
       </c>
       <c r="D23" s="2">
@@ -2210,51 +2444,86 @@
       <c r="H23" s="2">
         <v>0</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>39</v>
+      <c r="I23" s="2">
+        <v>0</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q23" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:18" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="J9:Q9"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="J11:Q11"/>
-    <mergeCell ref="I8:Q8"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="D3:Q3"/>
-    <mergeCell ref="I4:Q4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="I7:Q7"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="J6:Q6"/>
-    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="K9:R9"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="J8:R8"/>
+    <mergeCell ref="E2:R2"/>
+    <mergeCell ref="E3:R3"/>
+    <mergeCell ref="J4:R4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="J7:R7"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="H6:I6"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3 I4 I6:J6 B32:Q1048576 J10:N10 D11:H11 B11:B31 D12:Q31 B7:H10 B6:G6 B5:C5 E5 C4:F4 B2:D2">
+  <conditionalFormatting sqref="C3 J4 J6:K6 C32:R1048576 E11:I11 C11:C31 E12:R31 C7:I10 C6:H6 C5:D5 F5 D4:G4 C2:E2 K10:O10">
+    <cfRule type="cellIs" dxfId="60" priority="62" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="63" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="cellIs" dxfId="58" priority="60" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="61" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7">
+    <cfRule type="cellIs" dxfId="56" priority="58" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="59" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8">
+    <cfRule type="cellIs" dxfId="54" priority="56" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="57" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
     <cfRule type="cellIs" dxfId="52" priority="54" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -2262,211 +2531,211 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J10">
+    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="53" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P10">
+    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="51" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11">
+    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="49" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11">
+    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="47" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G6">
+    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="43" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:D31">
+    <cfRule type="cellIs" dxfId="38" priority="26" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="27" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:Q6">
+    <cfRule type="cellIs" dxfId="36" priority="38" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="39" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R5:R6">
+    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="37" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11:D15">
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="35" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:D20">
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21:D24">
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="31" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25:D26">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:D5 C1:R2 C4:R4 C3 E3:R3 F5:R5 C6:R1048576">
+    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11:E15">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16:E20">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16:F20">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",E5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="53" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="51" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",D3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:M5">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5:Q5">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O5:R5">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="47" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O10">
-    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="43" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="41" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I11">
-    <cfRule type="cellIs" dxfId="36" priority="38" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="39" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5:F6">
-    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="37" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4">
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="35" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27:C31">
-    <cfRule type="cellIs" dxfId="30" priority="18" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="19" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5:P6">
-    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="31" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q5:Q6">
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C15">
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16:C20">
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C24">
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25:C26">
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6:Q1048576 B5:C5 E5:Q5 B1:Q2 B4:Q4 B3 D3:Q3">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",B1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11:D15">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16:D20">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E16:E20">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",D5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",C3)))</formula>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Started work on schematic
</commit_message>
<xml_diff>
--- a/Doc/InstructionSet.xlsx
+++ b/Doc/InstructionSet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pschilk\home\Repos\psMCU\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18D5A13-9C4A-4F5C-A4B0-4A981EF6F8A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9F87C1-98AF-47F8-BC37-516DC5CB8667}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{2EEA8C3F-B9BC-45D7-931E-0DD5ED819EBA}"/>
+    <workbookView xWindow="29670" yWindow="7560" windowWidth="17040" windowHeight="6960" xr2:uid="{2EEA8C3F-B9BC-45D7-931E-0DD5ED819EBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="61">
   <si>
     <t>Instruction</t>
   </si>
@@ -208,6 +202,12 @@
   </si>
   <si>
     <t>COMPB</t>
+  </si>
+  <si>
+    <t>Return from Int.</t>
+  </si>
+  <si>
+    <t>RTRNI</t>
   </si>
 </sst>
 </file>
@@ -261,7 +261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -479,11 +479,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -542,6 +555,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -560,11 +576,98 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="61">
+  <dxfs count="73">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1006,7 +1109,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1302,13 +1405,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5890C83-178E-4CA4-8BC2-8D6953071DB1}">
-  <dimension ref="A1:T27"/>
+  <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.44140625" style="20" customWidth="1"/>
@@ -1394,22 +1497,22 @@
       <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="27"/>
       <c r="S2" t="s">
         <v>5</v>
       </c>
@@ -1430,22 +1533,22 @@
       <c r="D3" s="7">
         <v>0</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="25"/>
       <c r="S3" t="s">
         <v>6</v>
       </c>
@@ -1472,22 +1575,22 @@
       <c r="F4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="23" t="s">
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="25"/>
       <c r="S4" t="s">
         <v>11</v>
       </c>
@@ -1514,11 +1617,11 @@
       <c r="F5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
       <c r="J5" s="2" t="s">
         <v>37</v>
       </c>
@@ -1549,10 +1652,10 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C6" s="7">
         <v>0</v>
@@ -1560,39 +1663,55 @@
       <c r="D6" s="2">
         <v>0</v>
       </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="27"/>
-      <c r="J6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="22"/>
+      <c r="E6" s="29">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" s="21">
+        <v>0</v>
+      </c>
+      <c r="H6" s="21">
+        <v>0</v>
+      </c>
+      <c r="I6" s="21">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C7" s="7">
         <v>0</v>
@@ -1607,32 +1726,32 @@
         <v>0</v>
       </c>
       <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="24"/>
+        <v>1</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="28"/>
+      <c r="J7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="23"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C8" s="7">
         <v>0</v>
@@ -1650,29 +1769,29 @@
         <v>0</v>
       </c>
       <c r="H8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="25"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C9" s="7">
         <v>0</v>
@@ -1681,40 +1800,38 @@
         <v>0</v>
       </c>
       <c r="E9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K9" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="22"/>
+      <c r="J9" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="25"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C10" s="7">
         <v>0</v>
@@ -1732,41 +1849,31 @@
         <v>1</v>
       </c>
       <c r="H10" s="2">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2">
-        <v>1</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P10" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="22"/>
+        <v>1</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="23"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C11" s="7">
         <v>0</v>
@@ -1787,28 +1894,38 @@
         <v>0</v>
       </c>
       <c r="I11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="22"/>
+      <c r="K11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P11" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="23"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C12" s="7">
         <v>0</v>
@@ -1823,48 +1940,34 @@
         <v>1</v>
       </c>
       <c r="G12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" s="2">
-        <v>1</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R12" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="23"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="7">
         <v>0</v>
@@ -1885,7 +1988,7 @@
         <v>1</v>
       </c>
       <c r="I13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>33</v>
@@ -1917,10 +2020,10 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C14" s="7">
         <v>0</v>
@@ -1938,13 +2041,13 @@
         <v>0</v>
       </c>
       <c r="H14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="2">
-        <v>1</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>37</v>
+        <v>0</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>37</v>
@@ -1973,10 +2076,10 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="7">
         <v>0</v>
@@ -1997,7 +2100,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>37</v>
@@ -2029,10 +2132,10 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C16" s="7">
         <v>0</v>
@@ -2044,16 +2147,16 @@
         <v>0</v>
       </c>
       <c r="F16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>37</v>
@@ -2085,10 +2188,10 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C17" s="7">
         <v>0</v>
@@ -2109,10 +2212,10 @@
         <v>1</v>
       </c>
       <c r="I17" s="2">
-        <v>0</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>37</v>
@@ -2141,10 +2244,10 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="C18" s="7">
         <v>0</v>
@@ -2162,13 +2265,13 @@
         <v>1</v>
       </c>
       <c r="H18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="2">
-        <v>1</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>37</v>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>37</v>
@@ -2197,10 +2300,10 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C19" s="7">
         <v>0</v>
@@ -2221,7 +2324,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>37</v>
@@ -2253,10 +2356,10 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C20" s="7">
         <v>0</v>
@@ -2271,13 +2374,13 @@
         <v>0</v>
       </c>
       <c r="G20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>37</v>
@@ -2309,10 +2412,10 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C21" s="7">
         <v>0</v>
@@ -2333,7 +2436,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>37</v>
@@ -2365,10 +2468,10 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C22" s="7">
         <v>0</v>
@@ -2386,10 +2489,10 @@
         <v>0</v>
       </c>
       <c r="H22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>37</v>
@@ -2421,77 +2524,181 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2">
+        <v>1</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B24" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="7">
-        <v>0</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0</v>
-      </c>
-      <c r="F23" s="2">
-        <v>0</v>
-      </c>
-      <c r="G23" s="2">
-        <v>0</v>
-      </c>
-      <c r="H23" s="2">
-        <v>0</v>
-      </c>
-      <c r="I23" s="2">
-        <v>0</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R23" s="3" t="s">
+      <c r="C24" s="7">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R24" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:18" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="K9:R9"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="K11:R11"/>
-    <mergeCell ref="J8:R8"/>
+    <mergeCell ref="K10:R10"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="J9:R9"/>
     <mergeCell ref="E2:R2"/>
     <mergeCell ref="E3:R3"/>
     <mergeCell ref="J4:R4"/>
     <mergeCell ref="G4:I4"/>
-    <mergeCell ref="J7:R7"/>
+    <mergeCell ref="J8:R8"/>
     <mergeCell ref="G5:I5"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="K7:R7"/>
+    <mergeCell ref="H7:I7"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3 J4 J6:K6 C32:R1048576 E11:I11 C11:C31 E12:R31 C7:I10 C6:H6 C5:D5 F5 D4:G4 C2:E2 K10:O10">
+  <conditionalFormatting sqref="C3 J4 J7:K7 C33:R1048576 E12:I12 C12:C32 E13:R32 C8:I11 C7:H7 C5:D5 F5 D4:G4 C2:E2 K11:O11">
+    <cfRule type="cellIs" dxfId="72" priority="74" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="71" priority="75" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="cellIs" dxfId="70" priority="72" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="73" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8">
+    <cfRule type="cellIs" dxfId="68" priority="70" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="71" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9">
+    <cfRule type="cellIs" dxfId="66" priority="68" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="69" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="cellIs" dxfId="64" priority="66" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="67" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11">
+    <cfRule type="cellIs" dxfId="62" priority="64" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="65" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P11">
     <cfRule type="cellIs" dxfId="60" priority="62" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -2499,7 +2706,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
+  <conditionalFormatting sqref="K12">
     <cfRule type="cellIs" dxfId="58" priority="60" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -2507,7 +2714,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J7">
+  <conditionalFormatting sqref="J12">
     <cfRule type="cellIs" dxfId="56" priority="58" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -2515,7 +2722,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J8">
+  <conditionalFormatting sqref="G5 G7">
     <cfRule type="cellIs" dxfId="54" priority="56" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -2523,7 +2730,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
+  <conditionalFormatting sqref="C4">
     <cfRule type="cellIs" dxfId="52" priority="54" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -2531,156 +2738,158 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D28:D32">
+    <cfRule type="cellIs" dxfId="50" priority="38" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="39" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:Q7">
+    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="51" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R5:R7">
+    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="49" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:D16">
+    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="47" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17:D21">
+    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22:D25">
+    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="43" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26:D27">
+    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="41" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:D5 C1:R2 C4:R4 C3 E3:R3 F5:R5 C7:R1048576 J6:R6">
+    <cfRule type="containsText" dxfId="36" priority="37" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:E16">
+    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17:E21">
+    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17:F21">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",E5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",D3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:M6">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5:Q6">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O5:R6">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="53" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P10">
-    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="51" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="49" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="47" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5:G6">
-    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="43" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27:D31">
-    <cfRule type="cellIs" dxfId="38" priority="26" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="27" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J5:Q6">
-    <cfRule type="cellIs" dxfId="36" priority="38" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="39" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R5:R6">
-    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="37" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11:D15">
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="35" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16:D20">
-    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21:D24">
-    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="31" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D25:D26">
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5:D5 C1:R2 C4:R4 C3 E3:R3 F5:R5 C6:R1048576">
-    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",C1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11:E15">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E16:E20">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F16:F20">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F21">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
     <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -2688,41 +2897,41 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",E5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",D3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J5:M5">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N5:Q5">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O5:R5">
+  <conditionalFormatting sqref="C6:D6 F6">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:D6 F6:I6">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",C6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",E6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -2730,7 +2939,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J9">
+  <conditionalFormatting sqref="I6">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added new Instructions, not yet tested
 - Added PUSHA, PUSHB, PUSHM, POPA, POPB, POPM instead of PUSH/POP
 - Added ADDLA, ADDLB instead of ADDL
</commit_message>
<xml_diff>
--- a/Doc/InstructionSet.xlsx
+++ b/Doc/InstructionSet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pschilk\home\Repos\psMCU\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03878ECB-DFBC-4C35-AADB-BBA9F23A93F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4219F3B-17D9-40BB-9142-C8935AFE9B4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36510" yWindow="2130" windowWidth="17040" windowHeight="12975" xr2:uid="{2EEA8C3F-B9BC-45D7-931E-0DD5ED819EBA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2EEA8C3F-B9BC-45D7-931E-0DD5ED819EBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="67">
   <si>
     <t>Instruction</t>
   </si>
@@ -111,12 +111,6 @@
     <t>HALT</t>
   </si>
   <si>
-    <t>PUSH</t>
-  </si>
-  <si>
-    <t>POP</t>
-  </si>
-  <si>
     <t>RTRN</t>
   </si>
   <si>
@@ -153,9 +147,6 @@
     <t>[AND/OR/XOR](L)</t>
   </si>
   <si>
-    <t>ADD(L)</t>
-  </si>
-  <si>
     <t>COPY A/B</t>
   </si>
   <si>
@@ -208,6 +199,33 @@
   </si>
   <si>
     <t>LDD[P/R]</t>
+  </si>
+  <si>
+    <t>[Reserved]</t>
+  </si>
+  <si>
+    <t>POPA</t>
+  </si>
+  <si>
+    <t>PUSHA</t>
+  </si>
+  <si>
+    <t>POPB</t>
+  </si>
+  <si>
+    <t>PUSHB</t>
+  </si>
+  <si>
+    <t>POPM</t>
+  </si>
+  <si>
+    <t>PUSHM</t>
+  </si>
+  <si>
+    <t>ADD/ADDLA</t>
+  </si>
+  <si>
+    <t>ADDLB</t>
   </si>
 </sst>
 </file>
@@ -223,7 +241,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,6 +278,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -496,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -561,6 +585,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -579,11 +609,645 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="73">
+  <dxfs count="163">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1405,10 +2069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5890C83-178E-4CA4-8BC2-8D6953071DB1}">
-  <dimension ref="A1:T28"/>
+  <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A6" sqref="A6:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1427,7 +2091,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C1" s="11">
         <v>15</v>
@@ -1489,7 +2153,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="8">
         <v>1</v>
@@ -1497,22 +2161,22 @@
       <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="28"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="30"/>
       <c r="S2" t="s">
         <v>5</v>
       </c>
@@ -1525,7 +2189,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
@@ -1533,22 +2197,22 @@
       <c r="D3" s="7">
         <v>0</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="28"/>
       <c r="S3" t="s">
         <v>6</v>
       </c>
@@ -1561,7 +2225,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C4" s="7">
         <v>0</v>
@@ -1575,22 +2239,22 @@
       <c r="F4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="25" t="s">
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="26"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="28"/>
       <c r="S4" t="s">
         <v>11</v>
       </c>
@@ -1600,10 +2264,10 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C5" s="7">
         <v>0</v>
@@ -1617,46 +2281,44 @@
       <c r="F5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
       <c r="J5" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>56</v>
-      </c>
+      <c r="A6" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="33"/>
       <c r="C6" s="7">
         <v>0</v>
       </c>
@@ -1669,89 +2331,103 @@
       <c r="F6" s="5">
         <v>1</v>
       </c>
-      <c r="G6" s="21">
-        <v>0</v>
-      </c>
-      <c r="H6" s="21">
-        <v>0</v>
-      </c>
-      <c r="I6" s="21">
-        <v>0</v>
+      <c r="G6" s="23">
+        <v>1</v>
+      </c>
+      <c r="H6" s="23">
+        <v>1</v>
+      </c>
+      <c r="I6" s="23">
+        <v>1</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>41</v>
-      </c>
+      <c r="A7" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="33"/>
       <c r="C7" s="7">
         <v>0</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
       </c>
-      <c r="E7" s="2">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>1</v>
-      </c>
-      <c r="H7" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="29"/>
-      <c r="J7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="24"/>
+      <c r="E7" s="22">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+      <c r="G7" s="23">
+        <v>1</v>
+      </c>
+      <c r="H7" s="23">
+        <v>1</v>
+      </c>
+      <c r="I7" s="23">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
+      <c r="A8" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C8" s="7">
         <v>0</v>
@@ -1759,39 +2435,55 @@
       <c r="D8" s="2">
         <v>0</v>
       </c>
-      <c r="E8" s="2">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="26"/>
+      <c r="E8" s="22">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+      <c r="G8" s="23">
+        <v>1</v>
+      </c>
+      <c r="H8" s="23">
+        <v>0</v>
+      </c>
+      <c r="I8" s="23">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C9" s="7">
         <v>0</v>
@@ -1799,39 +2491,39 @@
       <c r="D9" s="2">
         <v>0</v>
       </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="25" t="s">
+      <c r="E9" s="22">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" s="23">
+        <v>1</v>
+      </c>
+      <c r="H9" s="23">
+        <v>0</v>
+      </c>
+      <c r="I9" s="23">
+        <v>0</v>
+      </c>
+      <c r="J9" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="26"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="28"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C10" s="7">
         <v>0</v>
@@ -1839,41 +2531,39 @@
       <c r="D10" s="2">
         <v>0</v>
       </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2">
-        <v>1</v>
-      </c>
-      <c r="H10" s="2">
-        <v>1</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="24"/>
+      <c r="E10" s="22">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="23">
+        <v>0</v>
+      </c>
+      <c r="H10" s="23">
+        <v>1</v>
+      </c>
+      <c r="I10" s="23">
+        <v>1</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="28"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C11" s="7">
         <v>0</v>
@@ -1881,51 +2571,55 @@
       <c r="D11" s="2">
         <v>0</v>
       </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>1</v>
-      </c>
-      <c r="G11" s="2">
-        <v>1</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2">
-        <v>1</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>21</v>
+      <c r="E11" s="22">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="23">
+        <v>0</v>
+      </c>
+      <c r="H11" s="23">
+        <v>1</v>
+      </c>
+      <c r="I11" s="23">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P11" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="24"/>
+        <v>35</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C12" s="7">
         <v>0</v>
@@ -1933,41 +2627,41 @@
       <c r="D12" s="2">
         <v>0</v>
       </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="23" t="s">
+      <c r="E12" s="22">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="23">
+        <v>0</v>
+      </c>
+      <c r="H12" s="23">
+        <v>0</v>
+      </c>
+      <c r="I12" s="23">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1</v>
+      </c>
+      <c r="K12" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="24"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="26"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C13" s="7">
         <v>0</v>
@@ -1975,55 +2669,55 @@
       <c r="D13" s="2">
         <v>0</v>
       </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2">
-        <v>1</v>
-      </c>
-      <c r="I13" s="2">
-        <v>1</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>33</v>
+      <c r="E13" s="22">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
+      <c r="G13" s="21">
+        <v>0</v>
+      </c>
+      <c r="H13" s="21">
+        <v>0</v>
+      </c>
+      <c r="I13" s="21">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="C14" s="7">
         <v>0</v>
@@ -2032,54 +2726,38 @@
         <v>0</v>
       </c>
       <c r="E14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="2">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2">
-        <v>1</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R14" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="31"/>
+      <c r="J14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="26"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C15" s="7">
         <v>0</v>
@@ -2088,54 +2766,38 @@
         <v>0</v>
       </c>
       <c r="E15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="2">
         <v>0</v>
       </c>
       <c r="H15" s="2">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2">
-        <v>1</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R15" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="28"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C16" s="7">
         <v>0</v>
@@ -2144,10 +2806,10 @@
         <v>0</v>
       </c>
       <c r="E16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="2">
         <v>0</v>
@@ -2155,43 +2817,27 @@
       <c r="H16" s="2">
         <v>0</v>
       </c>
-      <c r="I16" s="2">
-        <v>0</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R16" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="I16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="28"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C17" s="7">
         <v>0</v>
@@ -2203,7 +2849,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="2">
         <v>1</v>
@@ -2211,40 +2857,26 @@
       <c r="H17" s="2">
         <v>1</v>
       </c>
-      <c r="I17" s="2">
-        <v>1</v>
+      <c r="I17" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R17" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="K17" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="26"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>46</v>
@@ -2259,51 +2891,47 @@
         <v>0</v>
       </c>
       <c r="F18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="2">
         <v>1</v>
       </c>
       <c r="H18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="2">
-        <v>0</v>
-      </c>
-      <c r="J18" s="2">
-        <v>0</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>37</v>
+        <v>1</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R18" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="P18" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="26"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="C19" s="7">
         <v>0</v>
@@ -2315,7 +2943,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="2">
         <v>1</v>
@@ -2324,42 +2952,28 @@
         <v>0</v>
       </c>
       <c r="I19" s="2">
-        <v>1</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R19" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="26"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="C20" s="7">
         <v>0</v>
@@ -2371,51 +2985,51 @@
         <v>0</v>
       </c>
       <c r="F20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="2">
-        <v>0</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>37</v>
+        <v>1</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="C21" s="7">
         <v>0</v>
@@ -2427,7 +3041,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="2">
         <v>0</v>
@@ -2436,42 +3050,42 @@
         <v>1</v>
       </c>
       <c r="I21" s="2">
-        <v>1</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>37</v>
+        <v>0</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C22" s="7">
         <v>0</v>
@@ -2483,51 +3097,51 @@
         <v>0</v>
       </c>
       <c r="F22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="2">
         <v>0</v>
       </c>
       <c r="H22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C23" s="7">
         <v>0</v>
@@ -2539,7 +3153,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="2">
         <v>0</v>
@@ -2548,402 +3162,1171 @@
         <v>0</v>
       </c>
       <c r="I23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1</v>
+      </c>
+      <c r="I24" s="2">
+        <v>1</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R24" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2">
+        <v>1</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R25" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <v>1</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="7">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
+        <v>1</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R27" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="7">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R28" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="7">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R29" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="7">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2">
+        <v>1</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R30" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B31" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="7">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0</v>
-      </c>
-      <c r="F24" s="2">
-        <v>0</v>
-      </c>
-      <c r="G24" s="2">
-        <v>0</v>
-      </c>
-      <c r="H24" s="2">
-        <v>0</v>
-      </c>
-      <c r="I24" s="2">
-        <v>0</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R24" s="3" t="s">
-        <v>37</v>
+      <c r="C31" s="7">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R31" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="K10:R10"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="J9:R9"/>
+  <mergeCells count="15">
+    <mergeCell ref="K17:R17"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="K19:R19"/>
+    <mergeCell ref="J16:R16"/>
     <mergeCell ref="E2:R2"/>
     <mergeCell ref="E3:R3"/>
     <mergeCell ref="J4:R4"/>
     <mergeCell ref="G4:I4"/>
-    <mergeCell ref="J8:R8"/>
+    <mergeCell ref="J15:R15"/>
     <mergeCell ref="G5:I5"/>
-    <mergeCell ref="K7:R7"/>
-    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="K14:R14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J9:R9"/>
+    <mergeCell ref="J10:R10"/>
+    <mergeCell ref="K12:R12"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3 J4 J7:K7 C33:R1048576 E12:I12 C12:C32 E13:R32 C8:I11 C7:H7 C5:D5 F5 D4:G4 C2:E2 K11:O11">
-    <cfRule type="cellIs" dxfId="72" priority="74" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="75" operator="equal">
+  <conditionalFormatting sqref="C3 J4 J14:K14 C40:R1048576 E19:I19 C19:C39 E20:R39 C15:I18 C14:H14 C5:D5 F5 D4:G4 C2:E2 K18:O18">
+    <cfRule type="cellIs" dxfId="162" priority="176" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="161" priority="177" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="70" priority="72" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="73" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="68" priority="70" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="174" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="159" priority="175" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15">
+    <cfRule type="cellIs" dxfId="158" priority="172" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="157" priority="173" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16">
+    <cfRule type="cellIs" dxfId="156" priority="170" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="155" priority="171" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="cellIs" dxfId="154" priority="168" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="153" priority="169" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J18">
+    <cfRule type="cellIs" dxfId="152" priority="166" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="151" priority="167" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P18">
+    <cfRule type="cellIs" dxfId="150" priority="164" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="149" priority="165" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19">
+    <cfRule type="cellIs" dxfId="148" priority="162" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="147" priority="163" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J19">
+    <cfRule type="cellIs" dxfId="146" priority="160" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="145" priority="161" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5 G14">
+    <cfRule type="cellIs" dxfId="144" priority="158" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="143" priority="159" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="cellIs" dxfId="142" priority="156" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="141" priority="157" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35:D39">
+    <cfRule type="cellIs" dxfId="140" priority="140" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="139" priority="141" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:Q14">
+    <cfRule type="cellIs" dxfId="138" priority="152" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="137" priority="153" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R5:R14">
+    <cfRule type="cellIs" dxfId="136" priority="150" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="135" priority="151" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19:D23">
+    <cfRule type="cellIs" dxfId="134" priority="148" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="133" priority="149" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24:D28">
+    <cfRule type="cellIs" dxfId="132" priority="146" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="131" priority="147" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29:D32">
+    <cfRule type="cellIs" dxfId="130" priority="144" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="129" priority="145" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33:D34">
+    <cfRule type="cellIs" dxfId="128" priority="142" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="127" priority="143" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:D5 C1:R2 C4:R4 C3 E3:R3 F5:R5 C14:R1048576 J6:R13">
+    <cfRule type="containsText" dxfId="126" priority="139" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19:E23">
+    <cfRule type="cellIs" dxfId="125" priority="137" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="124" priority="138" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24:E28">
+    <cfRule type="cellIs" dxfId="123" priority="135" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="136" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29">
+    <cfRule type="cellIs" dxfId="121" priority="133" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="120" priority="134" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24:F28">
+    <cfRule type="cellIs" dxfId="119" priority="131" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="132" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F29">
+    <cfRule type="cellIs" dxfId="117" priority="129" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="130" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="115" priority="127" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="128" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="containsText" dxfId="113" priority="126" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",E5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="cellIs" dxfId="112" priority="124" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="111" priority="125" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="containsText" dxfId="110" priority="123" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",D3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:M13">
+    <cfRule type="cellIs" dxfId="109" priority="121" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="108" priority="122" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5:Q13">
+    <cfRule type="cellIs" dxfId="107" priority="119" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="120" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O5:R13">
+    <cfRule type="cellIs" dxfId="105" priority="117" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="104" priority="118" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17">
+    <cfRule type="cellIs" dxfId="103" priority="115" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="116" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:D13 F13">
+    <cfRule type="cellIs" dxfId="101" priority="113" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="100" priority="114" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13">
+    <cfRule type="cellIs" dxfId="99" priority="111" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="112" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:D13 F13:I13">
+    <cfRule type="containsText" dxfId="97" priority="110" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",C13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" dxfId="96" priority="108" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="109" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="containsText" dxfId="94" priority="107" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",E13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
+    <cfRule type="cellIs" dxfId="93" priority="105" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="106" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="cellIs" dxfId="91" priority="103" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="104" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:D12 F12">
+    <cfRule type="cellIs" dxfId="89" priority="101" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="102" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12">
+    <cfRule type="cellIs" dxfId="87" priority="99" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="100" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:D12 F12:I12">
+    <cfRule type="containsText" dxfId="85" priority="98" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",C12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" dxfId="84" priority="96" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="83" priority="97" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="containsText" dxfId="82" priority="95" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",E12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12">
+    <cfRule type="cellIs" dxfId="81" priority="93" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="94" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="cellIs" dxfId="79" priority="91" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="92" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:D11 F11">
+    <cfRule type="cellIs" dxfId="77" priority="89" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="90" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="cellIs" dxfId="75" priority="87" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="88" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:D11 F11:I11">
+    <cfRule type="containsText" dxfId="73" priority="86" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",C11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="cellIs" dxfId="72" priority="84" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="71" priority="85" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="containsText" dxfId="70" priority="83" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",E11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="cellIs" dxfId="69" priority="81" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="82" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" dxfId="67" priority="79" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="80" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
+    <cfRule type="cellIs" dxfId="65" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="10" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10">
+    <cfRule type="cellIs" dxfId="63" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K12">
+    <cfRule type="cellIs" dxfId="61" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:D10 F10">
+    <cfRule type="cellIs" dxfId="59" priority="65" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="66" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
+    <cfRule type="cellIs" dxfId="57" priority="63" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="64" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:D10 F10:I10">
+    <cfRule type="containsText" dxfId="55" priority="62" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",C10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="cellIs" dxfId="54" priority="60" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="61" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="containsText" dxfId="52" priority="59" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",E10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="cellIs" dxfId="51" priority="57" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="58" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10">
+    <cfRule type="cellIs" dxfId="49" priority="55" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="56" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:D9 F9">
+    <cfRule type="cellIs" dxfId="47" priority="53" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="54" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="cellIs" dxfId="45" priority="51" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="52" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:D9 F9:I9">
+    <cfRule type="containsText" dxfId="43" priority="50" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",C9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="cellIs" dxfId="42" priority="48" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="49" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="containsText" dxfId="40" priority="47" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",E9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
+    <cfRule type="cellIs" dxfId="37" priority="43" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="44" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:D8 F8">
+    <cfRule type="cellIs" dxfId="35" priority="41" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="42" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="40" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:D8 F8:I8">
+    <cfRule type="containsText" dxfId="31" priority="38" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",C8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="cellIs" dxfId="30" priority="36" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="37" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="containsText" dxfId="28" priority="35" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",E8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="34" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="cellIs" dxfId="25" priority="31" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="32" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:D7 F7">
+    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="30" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="cellIs" dxfId="21" priority="27" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="28" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:D7 F7:I7">
+    <cfRule type="containsText" dxfId="19" priority="26" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",C7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",E7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="20" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:D6 F6">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:D6 F6:I6">
+    <cfRule type="containsText" dxfId="7" priority="14" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",C6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="containsText" dxfId="4" priority="11" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",E6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="66" priority="68" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="69" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="64" priority="66" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="67" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="62" priority="64" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="65" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P11">
-    <cfRule type="cellIs" dxfId="60" priority="62" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="63" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="58" priority="60" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="61" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="56" priority="58" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="59" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5 G7">
-    <cfRule type="cellIs" dxfId="54" priority="56" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="57" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="52" priority="54" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="55" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28:D32">
-    <cfRule type="cellIs" dxfId="50" priority="38" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="39" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J5:Q7">
-    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="51" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R5:R7">
-    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="49" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12:D16">
-    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="47" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17:D21">
-    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22:D25">
-    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="43" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D26:D27">
-    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="41" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5:D5 C1:R2 C4:R4 C3 E3:R3 F5:R5 C7:R1048576 J6:R6">
-    <cfRule type="containsText" dxfId="36" priority="37" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",C1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12:E16">
-    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17:E21">
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F17:F21">
-    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F22">
-    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",E5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",D3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J5:M6">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N5:Q6">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O5:R6">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6:D6 F6">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6:D6 F6:I6">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",C6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",E6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>